<commit_message>
updated mockup added new project my Moni like loan Request form
</commit_message>
<xml_diff>
--- a/Nitesh/Loans4sme/EstimationAndCost.xlsx
+++ b/Nitesh/Loans4sme/EstimationAndCost.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="167">
   <si>
     <t>List to display all lender</t>
   </si>
@@ -265,6 +266,258 @@
   </si>
   <si>
     <t>Brief summary of Work</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Active Pre Lead</t>
+  </si>
+  <si>
+    <t>Borrower makes request.</t>
+  </si>
+  <si>
+    <t>Pre Lead Client Drop</t>
+  </si>
+  <si>
+    <t>Borrower or Systme Admin deletes loan request.</t>
+  </si>
+  <si>
+    <t>Active Stage 1 Lead</t>
+  </si>
+  <si>
+    <t>Background verification done Mandate letter generated</t>
+  </si>
+  <si>
+    <t>Stage 1 Reject</t>
+  </si>
+  <si>
+    <t>Sales rep. Rejects loan request at time of background verification.</t>
+  </si>
+  <si>
+    <t>Stage 1 Client Drop</t>
+  </si>
+  <si>
+    <t>Active Stage 2 Lead</t>
+  </si>
+  <si>
+    <t>Borrower upload document after successful background check</t>
+  </si>
+  <si>
+    <t>Stage 2 Reject</t>
+  </si>
+  <si>
+    <t>Credit checker reject loan req.</t>
+  </si>
+  <si>
+    <t>Stage 2 Client Drop</t>
+  </si>
+  <si>
+    <t>Active Listing</t>
+  </si>
+  <si>
+    <t>Credit checker approves loan request and loan request is forwareded to Lenders</t>
+  </si>
+  <si>
+    <t>Post Listing Client Drop</t>
+  </si>
+  <si>
+    <t>Lender Reject</t>
+  </si>
+  <si>
+    <t>Lender rejects</t>
+  </si>
+  <si>
+    <t>Active Sanction</t>
+  </si>
+  <si>
+    <t>Lender senction loan request</t>
+  </si>
+  <si>
+    <t>Sanctioned Client Drop</t>
+  </si>
+  <si>
+    <t>Sanctioned Lender Drop</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Disbursed</t>
+  </si>
+  <si>
+    <t>Active Repeat Listing</t>
+  </si>
+  <si>
+    <t>Stages</t>
+  </si>
+  <si>
+    <t>Document Checklist</t>
+  </si>
+  <si>
+    <t>KYC Documents</t>
+  </si>
+  <si>
+    <t>Certificate of Incorporation</t>
+  </si>
+  <si>
+    <t>MOA and AOA</t>
+  </si>
+  <si>
+    <t>Pan Card of Company</t>
+  </si>
+  <si>
+    <t>List of Directors</t>
+  </si>
+  <si>
+    <t>Pan Cards of all directors</t>
+  </si>
+  <si>
+    <t>Address Proof of all directors</t>
+  </si>
+  <si>
+    <t>Financial Statements</t>
+  </si>
+  <si>
+    <t>Audited financials for past three years</t>
+  </si>
+  <si>
+    <t>Audit Report and Tax Audit Report for last 3 years</t>
+  </si>
+  <si>
+    <t>Provisional financials for current year</t>
+  </si>
+  <si>
+    <t>Projected financials for loan term</t>
+  </si>
+  <si>
+    <t>Past Investments</t>
+  </si>
+  <si>
+    <t>Shareholding Pattern</t>
+  </si>
+  <si>
+    <t>Year-wise breakup of equity investment received (amount and investor)</t>
+  </si>
+  <si>
+    <t>Loans and Banking</t>
+  </si>
+  <si>
+    <t>List of all bank accounts maintained by the company</t>
+  </si>
+  <si>
+    <t>Bank Statements for ALL bank accounts for the last 12 months</t>
+  </si>
+  <si>
+    <t>Term sheets for all loans and credit facilities currently outstanding</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Company profile and brochure, if any</t>
+  </si>
+  <si>
+    <t>Latest investor presentation deck</t>
+  </si>
+  <si>
+    <t>Organisation Structure</t>
+  </si>
+  <si>
+    <t>Statutory Returns</t>
+  </si>
+  <si>
+    <t>Income Tax Returns for the last 2 years</t>
+  </si>
+  <si>
+    <t>VAT and/or service tax returns for the last 12 months</t>
+  </si>
+  <si>
+    <t>For Unsecured Business Loans or Invoice Discounting</t>
+  </si>
+  <si>
+    <t>List of Top Customers (Top 10 customers or top 50% sales)</t>
+  </si>
+  <si>
+    <t>Debtor Ageing Schedule</t>
+  </si>
+  <si>
+    <t>Customer contracts</t>
+  </si>
+  <si>
+    <t>Customer ledgers for top 10 customers</t>
+  </si>
+  <si>
+    <t>For PO based loan</t>
+  </si>
+  <si>
+    <t>Copy of the contract</t>
+  </si>
+  <si>
+    <t>Tender on which basis the contract was awarded</t>
+  </si>
+  <si>
+    <t>Milestones and expected payments/receipts for the project</t>
+  </si>
+  <si>
+    <t>Case studies - similar projects executed in the past</t>
+  </si>
+  <si>
+    <t>For term loan and leasing</t>
+  </si>
+  <si>
+    <t>Breakup of project cost</t>
+  </si>
+  <si>
+    <t>List of assets to be purchased</t>
+  </si>
+  <si>
+    <t>Technical specifications of proposed project</t>
+  </si>
+  <si>
+    <t>List of suppliers</t>
+  </si>
+  <si>
+    <t>Cash flow projections for the project</t>
+  </si>
+  <si>
+    <t>Confidential</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Subfolders under Public</t>
+  </si>
+  <si>
+    <t>KYC</t>
+  </si>
+  <si>
+    <t>Financials</t>
+  </si>
+  <si>
+    <t>Tax Returns</t>
+  </si>
+  <si>
+    <t>Bank Statements</t>
+  </si>
+  <si>
+    <t>PO and Invoice</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Lender 1 Additional Info</t>
+  </si>
+  <si>
+    <t>Lender 2 Additional Info</t>
+  </si>
+  <si>
+    <t>Lender 3 Additional Info</t>
+  </si>
+  <si>
+    <t>Folder Structure</t>
   </si>
 </sst>
 </file>
@@ -607,17 +860,17 @@
       <selection activeCell="G3" sqref="G3:G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="36.5703125" customWidth="1"/>
-    <col min="5" max="5" width="35.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="36.5546875" customWidth="1"/>
+    <col min="5" max="5" width="35.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" ht="30">
+    <row r="2" spans="3:17" ht="28.8">
       <c r="C2" t="s">
         <v>42</v>
       </c>
@@ -637,7 +890,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="3:17" ht="24.95" customHeight="1">
+    <row r="3" spans="3:17" ht="24.9" customHeight="1">
       <c r="C3" t="s">
         <v>43</v>
       </c>
@@ -664,7 +917,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="3:17" ht="24.95" customHeight="1">
+    <row r="4" spans="3:17" ht="24.9" customHeight="1">
       <c r="C4" t="s">
         <v>43</v>
       </c>
@@ -689,7 +942,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="3:17" ht="24.95" customHeight="1">
+    <row r="5" spans="3:17" ht="24.9" customHeight="1">
       <c r="C5" t="s">
         <v>43</v>
       </c>
@@ -714,7 +967,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="3:17" ht="24.95" customHeight="1">
+    <row r="6" spans="3:17" ht="24.9" customHeight="1">
       <c r="C6" t="s">
         <v>43</v>
       </c>
@@ -739,7 +992,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="3:17" ht="24.95" customHeight="1">
+    <row r="7" spans="3:17" ht="24.9" customHeight="1">
       <c r="C7" t="s">
         <v>43</v>
       </c>
@@ -766,7 +1019,7 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="3:17" ht="24.95" customHeight="1">
+    <row r="8" spans="3:17" ht="24.9" customHeight="1">
       <c r="C8" t="s">
         <v>43</v>
       </c>
@@ -791,7 +1044,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="3:17" ht="24.95" customHeight="1">
+    <row r="9" spans="3:17" ht="24.9" customHeight="1">
       <c r="C9" t="s">
         <v>43</v>
       </c>
@@ -816,7 +1069,7 @@
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
     </row>
-    <row r="10" spans="3:17" ht="24.95" customHeight="1">
+    <row r="10" spans="3:17" ht="24.9" customHeight="1">
       <c r="C10" t="s">
         <v>43</v>
       </c>
@@ -841,7 +1094,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="3:17" ht="24.95" customHeight="1">
+    <row r="11" spans="3:17" ht="24.9" customHeight="1">
       <c r="C11" t="s">
         <v>43</v>
       </c>
@@ -868,7 +1121,7 @@
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
     </row>
-    <row r="12" spans="3:17" ht="24.95" customHeight="1">
+    <row r="12" spans="3:17" ht="24.9" customHeight="1">
       <c r="C12" t="s">
         <v>43</v>
       </c>
@@ -893,7 +1146,7 @@
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
     </row>
-    <row r="13" spans="3:17" ht="24.95" customHeight="1">
+    <row r="13" spans="3:17" ht="24.9" customHeight="1">
       <c r="C13" t="s">
         <v>43</v>
       </c>
@@ -918,7 +1171,7 @@
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
     </row>
-    <row r="14" spans="3:17" ht="24.95" customHeight="1">
+    <row r="14" spans="3:17" ht="24.9" customHeight="1">
       <c r="C14" t="s">
         <v>43</v>
       </c>
@@ -997,7 +1250,7 @@
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
     </row>
-    <row r="17" spans="3:17" ht="24.95" customHeight="1">
+    <row r="17" spans="3:17" ht="24.9" customHeight="1">
       <c r="C17" t="s">
         <v>44</v>
       </c>
@@ -1026,7 +1279,7 @@
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
     </row>
-    <row r="18" spans="3:17" ht="24.95" customHeight="1">
+    <row r="18" spans="3:17" ht="24.9" customHeight="1">
       <c r="C18" t="s">
         <v>44</v>
       </c>
@@ -1055,7 +1308,7 @@
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="3:17" ht="24.95" customHeight="1">
+    <row r="19" spans="3:17" ht="24.9" customHeight="1">
       <c r="C19" t="s">
         <v>44</v>
       </c>
@@ -1136,7 +1389,7 @@
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
     </row>
-    <row r="22" spans="3:17" ht="30">
+    <row r="22" spans="3:17">
       <c r="C22" t="s">
         <v>43</v>
       </c>
@@ -1161,7 +1414,7 @@
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
     </row>
-    <row r="23" spans="3:17" ht="45">
+    <row r="23" spans="3:17" ht="43.2">
       <c r="C23" t="s">
         <v>43</v>
       </c>
@@ -1211,7 +1464,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="3:17" ht="45">
+    <row r="25" spans="3:17" ht="43.2">
       <c r="C25" t="s">
         <v>45</v>
       </c>
@@ -1265,7 +1518,7 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="3:17" ht="30">
+    <row r="27" spans="3:17" ht="28.8">
       <c r="C27" t="s">
         <v>45</v>
       </c>
@@ -1373,7 +1626,7 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="3:17" ht="45">
+    <row r="31" spans="3:17" ht="28.8">
       <c r="C31" t="s">
         <v>46</v>
       </c>
@@ -1481,7 +1734,7 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="3:17" ht="30">
+    <row r="35" spans="3:17">
       <c r="C35" t="s">
         <v>46</v>
       </c>
@@ -1508,7 +1761,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="3:17" ht="75">
+    <row r="36" spans="3:17" ht="72">
       <c r="C36" t="s">
         <v>53</v>
       </c>
@@ -1559,7 +1812,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="39" spans="3:17" ht="30">
+    <row r="39" spans="3:17" ht="28.8">
       <c r="C39" t="s">
         <v>53</v>
       </c>
@@ -1581,7 +1834,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="41" spans="3:17" ht="30">
+    <row r="41" spans="3:17">
       <c r="D41" s="1" t="s">
         <v>61</v>
       </c>
@@ -1607,17 +1860,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="F5:H23"/>
+  <dimension ref="F5:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="6" max="6" width="50.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="50.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="6:8">
@@ -1631,7 +1884,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="6:8" ht="30">
+    <row r="6" spans="6:8" ht="28.8">
       <c r="F6" s="1" t="s">
         <v>72</v>
       </c>
@@ -1642,7 +1895,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="6:8" ht="45">
+    <row r="7" spans="6:8" ht="28.8">
       <c r="F7" s="1" t="s">
         <v>73</v>
       </c>
@@ -1675,7 +1928,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="6:8" ht="30">
+    <row r="10" spans="6:8">
       <c r="F10" s="1" t="s">
         <v>64</v>
       </c>
@@ -1686,7 +1939,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="6:8" ht="45">
+    <row r="11" spans="6:8" ht="43.2">
       <c r="F11" s="1" t="s">
         <v>74</v>
       </c>
@@ -1697,7 +1950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="6:8" ht="30">
+    <row r="12" spans="6:8">
       <c r="F12" s="1" t="s">
         <v>75</v>
       </c>
@@ -1705,7 +1958,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="13" spans="6:8" ht="30">
+    <row r="13" spans="6:8" ht="28.8">
       <c r="F13" s="1" t="s">
         <v>76</v>
       </c>
@@ -1716,7 +1969,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="6:8" ht="45">
+    <row r="14" spans="6:8" ht="43.2">
       <c r="F14" s="1" t="s">
         <v>77</v>
       </c>
@@ -1727,7 +1980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="6:8" ht="30">
+    <row r="15" spans="6:8" ht="28.8">
       <c r="F15" s="1" t="s">
         <v>68</v>
       </c>
@@ -1749,31 +2002,43 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="6:7">
+    <row r="19" spans="6:9">
       <c r="F19" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G19" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="20" spans="6:7">
+      <c r="H19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="6:9">
       <c r="F20" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G20" s="2">
         <v>43001</v>
       </c>
-    </row>
-    <row r="21" spans="6:7">
+      <c r="H20">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="21" spans="6:9">
       <c r="F21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="3">
         <v>43010</v>
       </c>
-    </row>
-    <row r="22" spans="6:7">
+      <c r="H21">
+        <v>35000</v>
+      </c>
+      <c r="I21">
+        <v>59000</v>
+      </c>
+    </row>
+    <row r="22" spans="6:9">
       <c r="F22" s="1" t="s">
         <v>80</v>
       </c>
@@ -1781,7 +2046,7 @@
         <v>43023</v>
       </c>
     </row>
-    <row r="23" spans="6:7">
+    <row r="23" spans="6:9">
       <c r="F23" s="1"/>
     </row>
   </sheetData>
@@ -1792,11 +2057,382 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="H9:Q52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="9" spans="8:17">
+      <c r="H9" t="s">
+        <v>110</v>
+      </c>
+      <c r="N9" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11" spans="8:17">
+      <c r="H11" t="s">
+        <v>84</v>
+      </c>
+      <c r="I11" t="s">
+        <v>85</v>
+      </c>
+      <c r="N11" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="8:17">
+      <c r="H12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" t="s">
+        <v>87</v>
+      </c>
+      <c r="N12" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="8:17">
+      <c r="H13" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" t="s">
+        <v>89</v>
+      </c>
+      <c r="N13" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="8:17">
+      <c r="H14" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" t="s">
+        <v>91</v>
+      </c>
+      <c r="N14" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="8:17">
+      <c r="H15" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" t="s">
+        <v>87</v>
+      </c>
+      <c r="N15" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="8:17">
+      <c r="H16" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" t="s">
+        <v>94</v>
+      </c>
+      <c r="N16" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="8:17">
+      <c r="H17" t="s">
+        <v>95</v>
+      </c>
+      <c r="I17" t="s">
+        <v>96</v>
+      </c>
+      <c r="N17" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="8:17">
+      <c r="H18" t="s">
+        <v>97</v>
+      </c>
+      <c r="I18" t="s">
+        <v>87</v>
+      </c>
+      <c r="N18" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="8:17">
+      <c r="H19" t="s">
+        <v>98</v>
+      </c>
+      <c r="I19" t="s">
+        <v>99</v>
+      </c>
+      <c r="N19" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="8:17">
+      <c r="H20" t="s">
+        <v>100</v>
+      </c>
+      <c r="I20" t="s">
+        <v>87</v>
+      </c>
+      <c r="N20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="8:17">
+      <c r="H21" t="s">
+        <v>101</v>
+      </c>
+      <c r="I21" t="s">
+        <v>102</v>
+      </c>
+      <c r="N21" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="8:17">
+      <c r="H22" t="s">
+        <v>103</v>
+      </c>
+      <c r="I22" t="s">
+        <v>104</v>
+      </c>
+      <c r="N22" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="8:17">
+      <c r="H23" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" t="s">
+        <v>87</v>
+      </c>
+      <c r="N23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="8:17">
+      <c r="H24" t="s">
+        <v>106</v>
+      </c>
+      <c r="I24" t="s">
+        <v>107</v>
+      </c>
+      <c r="N24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="8:17">
+      <c r="H25" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" t="s">
+        <v>107</v>
+      </c>
+      <c r="N25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="8:17">
+      <c r="H26" t="s">
+        <v>109</v>
+      </c>
+      <c r="I26" t="s">
+        <v>107</v>
+      </c>
+      <c r="N26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="8:17">
+      <c r="N27" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="8:17">
+      <c r="N28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="8:17">
+      <c r="N29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="8:17">
+      <c r="N30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="8:17">
+      <c r="N31" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="8:17">
+      <c r="N32" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="14:14">
+      <c r="N33" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="14:14">
+      <c r="N34" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="14:14">
+      <c r="N35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="14:14">
+      <c r="N36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="14:14">
+      <c r="N37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="14:14">
+      <c r="N38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="14:14">
+      <c r="N39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="14:14">
+      <c r="N40" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="14:14">
+      <c r="N41" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="14:14">
+      <c r="N42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="14:14">
+      <c r="N43" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="14:14">
+      <c r="N44" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="45" spans="14:14">
+      <c r="N45" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="14:14">
+      <c r="N46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="14:14">
+      <c r="N47" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="48" spans="14:14">
+      <c r="N48" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="49" spans="14:14">
+      <c r="N49" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="14:14">
+      <c r="N50" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="51" spans="14:14">
+      <c r="N51" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="14:14">
+      <c r="N52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>